<commit_message>
Interim committ - changes to autonomous variables speed
</commit_message>
<xml_diff>
--- a/docs/autonomous_distance_trials.xlsx
+++ b/docs/autonomous_distance_trials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="9495" windowHeight="5895" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="9495" windowHeight="5895"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>trial</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>right circle</t>
+  </si>
+  <si>
+    <t>skewed to right</t>
   </si>
 </sst>
 </file>
@@ -409,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -762,7 +765,7 @@
         <v>16</v>
       </c>
       <c r="K10">
-        <f t="shared" ref="K9:K12" si="3">E10+F10</f>
+        <f t="shared" ref="K10:K12" si="3">E10+F10</f>
         <v>-126</v>
       </c>
       <c r="L10">
@@ -783,23 +786,42 @@
       <c r="D11">
         <v>4.8</v>
       </c>
+      <c r="I11">
+        <v>19.5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
       <c r="K11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.0625</v>
       </c>
     </row>
     <row r="12" spans="1:12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>6.9999999999999994E-5</v>
+      </c>
+      <c r="D12">
+        <f>20/4</f>
+        <v>5</v>
+      </c>
       <c r="K12">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="L12" t="e">
+      <c r="L12">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -811,7 +833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>